<commit_message>
initial release (pre-release) first prod version
</commit_message>
<xml_diff>
--- a/users.xlsx
+++ b/users.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="220">
   <si>
     <t>Last name</t>
   </si>
@@ -40,382 +40,457 @@
     <t>Passport number</t>
   </si>
   <si>
-    <t>HATICE</t>
-  </si>
-  <si>
-    <t>SELVIYE</t>
+    <t>KADIR KAAN</t>
+  </si>
+  <si>
+    <t>YIGIT</t>
+  </si>
+  <si>
+    <t>SERDAL</t>
+  </si>
+  <si>
+    <t>FULYA</t>
+  </si>
+  <si>
+    <t>TOLGA</t>
+  </si>
+  <si>
+    <t>ERMAN</t>
+  </si>
+  <si>
+    <t>ERDEM</t>
+  </si>
+  <si>
+    <t>UMUT</t>
+  </si>
+  <si>
+    <t>NAZLICAN</t>
+  </si>
+  <si>
+    <t>TANSU</t>
   </si>
   <si>
     <t>FILIZ</t>
   </si>
   <si>
-    <t>ECE</t>
-  </si>
-  <si>
-    <t>KADIR KAAN</t>
-  </si>
-  <si>
-    <t>IBRAHIM</t>
-  </si>
-  <si>
-    <t>OKAN</t>
-  </si>
-  <si>
-    <t>ILKER</t>
-  </si>
-  <si>
-    <t>ZEYNEP</t>
-  </si>
-  <si>
-    <t>SENA</t>
-  </si>
-  <si>
-    <t>SERDAL</t>
-  </si>
-  <si>
-    <t>FULYA</t>
+    <t>EROL</t>
+  </si>
+  <si>
+    <t>ENGIN</t>
+  </si>
+  <si>
+    <t>SAMET</t>
+  </si>
+  <si>
+    <t>DUYGU</t>
+  </si>
+  <si>
+    <t>AY</t>
+  </si>
+  <si>
+    <t>BOZER</t>
+  </si>
+  <si>
+    <t>KARADAG</t>
+  </si>
+  <si>
+    <t>SIBEL</t>
+  </si>
+  <si>
+    <t>TASTEKIN</t>
+  </si>
+  <si>
+    <t>KAPTAN</t>
+  </si>
+  <si>
+    <t>TABANLI</t>
+  </si>
+  <si>
+    <t>OZEL</t>
+  </si>
+  <si>
+    <t>DENIZ</t>
+  </si>
+  <si>
+    <t>ANIL</t>
+  </si>
+  <si>
+    <t>SAVAS</t>
+  </si>
+  <si>
+    <t>ASLAN</t>
+  </si>
+  <si>
+    <t>GURBUZ</t>
+  </si>
+  <si>
+    <t>AKTAS</t>
+  </si>
+  <si>
+    <t>AKBULUT</t>
+  </si>
+  <si>
+    <t>IRESAR</t>
+  </si>
+  <si>
+    <t>DURMAZ</t>
+  </si>
+  <si>
+    <t>CINAR</t>
+  </si>
+  <si>
+    <t>AHMETLER</t>
+  </si>
+  <si>
+    <t>SEVEN</t>
+  </si>
+  <si>
+    <t>KOKSAL</t>
+  </si>
+  <si>
+    <t>GOKKURT</t>
+  </si>
+  <si>
+    <t>ULU</t>
+  </si>
+  <si>
+    <t>TEMIZ</t>
+  </si>
+  <si>
+    <t>CAN</t>
+  </si>
+  <si>
+    <t>AYER</t>
+  </si>
+  <si>
+    <t>SABUNCUOGLU</t>
+  </si>
+  <si>
+    <t>GOKHAN</t>
+  </si>
+  <si>
+    <t>RECEP</t>
+  </si>
+  <si>
+    <t>EMEL</t>
+  </si>
+  <si>
+    <t>PARLAKSU</t>
+  </si>
+  <si>
+    <t>AHMET</t>
+  </si>
+  <si>
+    <t>SERAP</t>
+  </si>
+  <si>
+    <t>MURAT</t>
+  </si>
+  <si>
+    <t>CIGDEM</t>
+  </si>
+  <si>
+    <t>OZLEM</t>
+  </si>
+  <si>
+    <t>MUHAMMED</t>
+  </si>
+  <si>
+    <t>BURCU</t>
+  </si>
+  <si>
+    <t>GOKBERK</t>
+  </si>
+  <si>
+    <t>GORKEM</t>
+  </si>
+  <si>
+    <t>EYLUL</t>
+  </si>
+  <si>
+    <t>MELIKE AYCIN</t>
+  </si>
+  <si>
+    <t>SEZER</t>
+  </si>
+  <si>
+    <t>LEVENT</t>
+  </si>
+  <si>
+    <t>1995-09-05</t>
+  </si>
+  <si>
+    <t>1987-11-02</t>
+  </si>
+  <si>
+    <t>1979-01-01</t>
+  </si>
+  <si>
+    <t>1983-11-15</t>
+  </si>
+  <si>
+    <t>1995-06-04</t>
+  </si>
+  <si>
+    <t>1987-05-15</t>
+  </si>
+  <si>
+    <t>1985-01-17</t>
+  </si>
+  <si>
+    <t>2000-03-04</t>
+  </si>
+  <si>
+    <t>2001-07-13</t>
+  </si>
+  <si>
+    <t>1996-02-28</t>
+  </si>
+  <si>
+    <t>1979-05-25</t>
+  </si>
+  <si>
+    <t>1977-11-02</t>
+  </si>
+  <si>
+    <t>1979-09-22</t>
+  </si>
+  <si>
+    <t>1994-04-15</t>
+  </si>
+  <si>
+    <t>1990-09-10</t>
+  </si>
+  <si>
+    <t>1985-03-08</t>
+  </si>
+  <si>
+    <t>1982-06-01</t>
+  </si>
+  <si>
+    <t>1982-07-12</t>
+  </si>
+  <si>
+    <t>1969-07-02</t>
+  </si>
+  <si>
+    <t>1982-12-09</t>
+  </si>
+  <si>
+    <t>1979-04-20</t>
+  </si>
+  <si>
+    <t>1978-09-29</t>
+  </si>
+  <si>
+    <t>1978-07-05</t>
+  </si>
+  <si>
+    <t>1995-01-21</t>
+  </si>
+  <si>
+    <t>2004-03-09</t>
+  </si>
+  <si>
+    <t>1993-02-21</t>
+  </si>
+  <si>
+    <t>1988-01-23</t>
+  </si>
+  <si>
+    <t>2006-08-28</t>
+  </si>
+  <si>
+    <t>1977-08-25</t>
+  </si>
+  <si>
+    <t>1997-01-01</t>
+  </si>
+  <si>
+    <t>1970-04-20</t>
+  </si>
+  <si>
+    <t>ISTANBUL</t>
+  </si>
+  <si>
+    <t>SILIVRI</t>
+  </si>
+  <si>
+    <t>ANTALYA</t>
+  </si>
+  <si>
+    <t>BAKIRKOY</t>
+  </si>
+  <si>
+    <t>CORLU</t>
+  </si>
+  <si>
+    <t>BAYRAMPASA</t>
+  </si>
+  <si>
+    <t>TEKIRDAG</t>
+  </si>
+  <si>
+    <t>BERLIN</t>
+  </si>
+  <si>
+    <t>ESKISEHIR</t>
+  </si>
+  <si>
+    <t>BANARLI</t>
+  </si>
+  <si>
+    <t>KOVANCILAR</t>
+  </si>
+  <si>
+    <t>BURSA</t>
+  </si>
+  <si>
+    <t>NILUFER</t>
+  </si>
+  <si>
+    <t>INEGOL</t>
+  </si>
+  <si>
+    <t>MURATLI</t>
+  </si>
+  <si>
+    <t>ESIN</t>
+  </si>
+  <si>
+    <t>FATMA</t>
+  </si>
+  <si>
+    <t>HULYA</t>
+  </si>
+  <si>
+    <t>AYSE</t>
+  </si>
+  <si>
+    <t>NERIMAN</t>
+  </si>
+  <si>
+    <t>SEMRA</t>
+  </si>
+  <si>
+    <t>HACCEGUL</t>
+  </si>
+  <si>
+    <t>SANEM GAMZE</t>
+  </si>
+  <si>
+    <t>EMIBNE</t>
+  </si>
+  <si>
+    <t>MERYEM</t>
+  </si>
+  <si>
+    <t>SERIFE</t>
+  </si>
+  <si>
+    <t>NURIYE</t>
+  </si>
+  <si>
+    <t>HUSNIYE</t>
+  </si>
+  <si>
+    <t>SELIME</t>
+  </si>
+  <si>
+    <t>FEVZIYE</t>
+  </si>
+  <si>
+    <t>NEJLA</t>
+  </si>
+  <si>
+    <t>NADIYE</t>
+  </si>
+  <si>
+    <t>NACIYE</t>
+  </si>
+  <si>
+    <t>SEVGI</t>
+  </si>
+  <si>
+    <t>NURCAN</t>
+  </si>
+  <si>
+    <t>GULCIN</t>
+  </si>
+  <si>
+    <t>YUKSEL</t>
+  </si>
+  <si>
+    <t>EMINE</t>
+  </si>
+  <si>
+    <t>NIHAT</t>
+  </si>
+  <si>
+    <t>ONDER</t>
+  </si>
+  <si>
+    <t>ALI</t>
+  </si>
+  <si>
+    <t>DAGHAN</t>
   </si>
   <si>
     <t>SEFA</t>
   </si>
   <si>
-    <t>TOLGA</t>
-  </si>
-  <si>
-    <t>ERMAN</t>
-  </si>
-  <si>
-    <t>ERDEM</t>
-  </si>
-  <si>
-    <t>GURKAN</t>
-  </si>
-  <si>
-    <t>UMUT</t>
-  </si>
-  <si>
-    <t>NAZLICAN</t>
-  </si>
-  <si>
-    <t>TANSU</t>
-  </si>
-  <si>
-    <t>EROL</t>
-  </si>
-  <si>
-    <t>ENGIN</t>
-  </si>
-  <si>
-    <t>SAMET</t>
-  </si>
-  <si>
-    <t>DUYGU</t>
-  </si>
-  <si>
-    <t>YUKSELOGLU</t>
-  </si>
-  <si>
-    <t>ARACI</t>
-  </si>
-  <si>
-    <t>TEKCAN</t>
-  </si>
-  <si>
-    <t>AKBULUT</t>
-  </si>
-  <si>
-    <t>ORHUN</t>
-  </si>
-  <si>
-    <t>TEMURLENK</t>
-  </si>
-  <si>
-    <t>NAS</t>
-  </si>
-  <si>
-    <t>CICEK</t>
-  </si>
-  <si>
-    <t>IRESAR</t>
+    <t>SABRI</t>
+  </si>
+  <si>
+    <t>RAMAZAN</t>
+  </si>
+  <si>
+    <t>SERAFETTIN</t>
+  </si>
+  <si>
+    <t>BEYTULLAH</t>
+  </si>
+  <si>
+    <t>OSMAN</t>
   </si>
   <si>
     <t>ERGIN</t>
   </si>
   <si>
-    <t>DURMAZ</t>
-  </si>
-  <si>
-    <t>CINAR</t>
-  </si>
-  <si>
-    <t>AHMETLER</t>
-  </si>
-  <si>
-    <t>SEVEN</t>
-  </si>
-  <si>
-    <t>KOKSAL</t>
-  </si>
-  <si>
-    <t>TURETKEN</t>
-  </si>
-  <si>
-    <t>GOKKURT</t>
-  </si>
-  <si>
-    <t>ULU</t>
-  </si>
-  <si>
-    <t>OZCAN</t>
-  </si>
-  <si>
-    <t>TEMIZ</t>
-  </si>
-  <si>
-    <t>CAN</t>
-  </si>
-  <si>
-    <t>AYER</t>
-  </si>
-  <si>
-    <t>SABUNCUOGLU</t>
-  </si>
-  <si>
-    <t>1957-10-01</t>
-  </si>
-  <si>
-    <t>1962-09-05</t>
-  </si>
-  <si>
-    <t>1988-08-27</t>
-  </si>
-  <si>
-    <t>1990-01-23</t>
-  </si>
-  <si>
-    <t>1995-09-05</t>
-  </si>
-  <si>
-    <t>1935-12-31</t>
-  </si>
-  <si>
-    <t>1993-03-10</t>
-  </si>
-  <si>
-    <t>1979-10-07</t>
-  </si>
-  <si>
-    <t>1995-10-18</t>
-  </si>
-  <si>
-    <t>1998-09-26</t>
-  </si>
-  <si>
-    <t>1979-01-01</t>
-  </si>
-  <si>
-    <t>1983-11-15</t>
-  </si>
-  <si>
-    <t>1995-06-04</t>
-  </si>
-  <si>
-    <t>1987-05-15</t>
-  </si>
-  <si>
-    <t>1985-01-17</t>
-  </si>
-  <si>
-    <t>1979-01-10</t>
-  </si>
-  <si>
-    <t>2000-03-04</t>
-  </si>
-  <si>
-    <t>2001-07-13</t>
-  </si>
-  <si>
-    <t>1996-02-28</t>
-  </si>
-  <si>
-    <t>1979-05-25</t>
-  </si>
-  <si>
-    <t>1977-11-02</t>
-  </si>
-  <si>
-    <t>1979-09-22</t>
-  </si>
-  <si>
-    <t>1994-04-15</t>
-  </si>
-  <si>
-    <t>1990-09-10</t>
-  </si>
-  <si>
-    <t>SILIVRI</t>
-  </si>
-  <si>
-    <t>UZUNKOPRU</t>
-  </si>
-  <si>
-    <t>KADIKOY</t>
-  </si>
-  <si>
-    <t>ISTANBUL</t>
-  </si>
-  <si>
-    <t>SINCAN</t>
-  </si>
-  <si>
-    <t>CORLU</t>
-  </si>
-  <si>
-    <t>TEKIRDAG</t>
-  </si>
-  <si>
-    <t>ANTALYA</t>
-  </si>
-  <si>
-    <t>BAKIRKOY</t>
-  </si>
-  <si>
-    <t>IZMIT</t>
-  </si>
-  <si>
-    <t>BAYRAMPASA</t>
-  </si>
-  <si>
-    <t>FATMA</t>
-  </si>
-  <si>
-    <t>REMZIYE</t>
-  </si>
-  <si>
-    <t>HAYRIYE</t>
-  </si>
-  <si>
-    <t>ESIN</t>
-  </si>
-  <si>
-    <t>FERAH</t>
-  </si>
-  <si>
-    <t>HAMIYET</t>
-  </si>
-  <si>
-    <t>NIGAR</t>
-  </si>
-  <si>
-    <t>HULYA</t>
-  </si>
-  <si>
-    <t>AYSE</t>
-  </si>
-  <si>
-    <t>NERIMAN</t>
-  </si>
-  <si>
-    <t>SEMRA</t>
-  </si>
-  <si>
-    <t>NEVIN</t>
-  </si>
-  <si>
-    <t>HACCEGUL</t>
-  </si>
-  <si>
-    <t>SANEM GAMZE</t>
-  </si>
-  <si>
-    <t>MERYEM</t>
-  </si>
-  <si>
-    <t>EMIBNE</t>
-  </si>
-  <si>
-    <t>SERIFE</t>
-  </si>
-  <si>
-    <t>NAZMI</t>
-  </si>
-  <si>
-    <t>HAMIT</t>
-  </si>
-  <si>
-    <t>NIHAT</t>
-  </si>
-  <si>
     <t>RAHMI</t>
   </si>
   <si>
-    <t>ERBIL</t>
-  </si>
-  <si>
-    <t>SAHIN</t>
-  </si>
-  <si>
-    <t>ONDER</t>
-  </si>
-  <si>
-    <t>AYHAN</t>
-  </si>
-  <si>
-    <t>ALI</t>
-  </si>
-  <si>
-    <t>DAGHAN</t>
-  </si>
-  <si>
-    <t>AHMET</t>
-  </si>
-  <si>
-    <t>SABRI</t>
-  </si>
-  <si>
-    <t>RAMAZAN</t>
-  </si>
-  <si>
-    <t>METIN</t>
-  </si>
-  <si>
-    <t>BEYTULLAH</t>
-  </si>
-  <si>
-    <t>SERAFETTIN</t>
-  </si>
-  <si>
-    <t>OSMAN</t>
-  </si>
-  <si>
-    <t>HATICEYUKSELOGLU57@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>SELVIYEARACI62@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>FILIZTEKCAN-4072@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>ECEAKBLT@HOTMAIL.COM</t>
+    <t>IHSAN</t>
+  </si>
+  <si>
+    <t>KAMIL</t>
+  </si>
+  <si>
+    <t>CEVDET</t>
+  </si>
+  <si>
+    <t>SELAMETTIN</t>
+  </si>
+  <si>
+    <t>MEHMET</t>
+  </si>
+  <si>
+    <t>VESAL</t>
+  </si>
+  <si>
+    <t>MEMDUH</t>
+  </si>
+  <si>
+    <t>HALDUN</t>
+  </si>
+  <si>
+    <t>GONUL</t>
   </si>
   <si>
     <t>KAANAKBLT@HOTMAILCOM</t>
   </si>
   <si>
-    <t>SERHAT.ORHUN@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>OKANTEMURLENK05@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>NASILKER5959@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>ZYNPIRSR@GMAIL.COM</t>
-  </si>
-  <si>
-    <t>SENAIRESAR@GMAIL.COM</t>
+    <t>YIGITIRESAR@GMNAIL.COM</t>
   </si>
   <si>
     <t>SERDALDURMAZ@GMAIL.COM</t>
@@ -433,9 +508,6 @@
     <t>ERDEMMKOKSAL@GMAIL.COM</t>
   </si>
   <si>
-    <t>GURKANTURETKEN@GMAILCOM</t>
-  </si>
-  <si>
     <t>UMUTGOKKURT.1610@GMAIL.COM</t>
   </si>
   <si>
@@ -460,34 +532,61 @@
     <t>DUYGUIRESAR@HOTMAIL.COM</t>
   </si>
   <si>
-    <t>U11684195</t>
-  </si>
-  <si>
-    <t>U26338608</t>
-  </si>
-  <si>
-    <t>U36636720</t>
-  </si>
-  <si>
-    <t>U15963706</t>
+    <t>HANOGLUILETISIM@HOTMAIL.COM</t>
+  </si>
+  <si>
+    <t>RECEPBOZER@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>EKARADAG@ULUDAG.EDU.TR</t>
+  </si>
+  <si>
+    <t>PARLAKSUSIBEL@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>AHMETTASTEKIN1@HOTMAIL.COM</t>
+  </si>
+  <si>
+    <t>SERAP-TABANLI@HOTMAIL.COM</t>
+  </si>
+  <si>
+    <t>MURAT_TAB@YAHOO.COM</t>
+  </si>
+  <si>
+    <t>UYARCIGDEM@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>OZLEM.BILMEZ@HOTMAIL.COM</t>
+  </si>
+  <si>
+    <t>MHD_DENIZ@HOTMAIL.COM</t>
+  </si>
+  <si>
+    <t>BURCUDENIZ2046@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>GOKBERKANL@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>GORKEMANILL@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>EYLULANIL5@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>DOFSET@DOFSET.COM.TR</t>
+  </si>
+  <si>
+    <t>SEZERGURBUZ599@GMAIL.COM</t>
+  </si>
+  <si>
+    <t>ALEYNAOZKAN59@HOTMAIL.COM</t>
   </si>
   <si>
     <t>U27690632</t>
   </si>
   <si>
-    <t>U25290678</t>
-  </si>
-  <si>
-    <t>U23862611</t>
-  </si>
-  <si>
-    <t>U35136644</t>
-  </si>
-  <si>
-    <t>A23S67998</t>
-  </si>
-  <si>
-    <t>A31V74286</t>
+    <t>A04M83815</t>
   </si>
   <si>
     <t>U27032147</t>
@@ -505,9 +604,6 @@
     <t>U28831754</t>
   </si>
   <si>
-    <t>U27724090</t>
-  </si>
-  <si>
     <t>U32866768</t>
   </si>
   <si>
@@ -532,19 +628,52 @@
     <t>A35G14169</t>
   </si>
   <si>
-    <t>AKBULUTKINALITOPUK</t>
-  </si>
-  <si>
-    <t>YIGIT</t>
-  </si>
-  <si>
-    <t>1987-11-02</t>
-  </si>
-  <si>
-    <t>YIGITIRESAR@GMNAIL.COM</t>
-  </si>
-  <si>
-    <t>A04M83815</t>
+    <t>U15995271</t>
+  </si>
+  <si>
+    <t>S21219154</t>
+  </si>
+  <si>
+    <t>S35090082</t>
+  </si>
+  <si>
+    <t>U33059669</t>
+  </si>
+  <si>
+    <t>U31470613</t>
+  </si>
+  <si>
+    <t>U36757398</t>
+  </si>
+  <si>
+    <t>U20246456</t>
+  </si>
+  <si>
+    <t>U29633310</t>
+  </si>
+  <si>
+    <t>U33884490</t>
+  </si>
+  <si>
+    <t>U36715807</t>
+  </si>
+  <si>
+    <t>U33007568</t>
+  </si>
+  <si>
+    <t>U29343841</t>
+  </si>
+  <si>
+    <t>U33311108</t>
+  </si>
+  <si>
+    <t>U25552963</t>
+  </si>
+  <si>
+    <t>U33024373</t>
+  </si>
+  <si>
+    <t>U23189306</t>
   </si>
 </sst>
 </file>
@@ -909,22 +1038,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="33" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -955,652 +1083,886 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
       <c r="D2" t="s">
-        <v>79</v>
+        <v>105</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="F2" t="s">
-        <v>107</v>
+        <v>147</v>
       </c>
       <c r="G2" t="s">
-        <v>124</v>
+        <v>172</v>
       </c>
       <c r="H2" t="s">
-        <v>148</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>106</v>
       </c>
       <c r="E3" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="F3" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="G3" t="s">
-        <v>125</v>
+        <v>173</v>
       </c>
       <c r="H3" t="s">
-        <v>149</v>
+        <v>205</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>34</v>
+        <v>52</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>83</v>
       </c>
       <c r="D4" t="s">
-        <v>81</v>
+        <v>106</v>
       </c>
       <c r="E4" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
       <c r="F4" t="s">
-        <v>50</v>
+        <v>148</v>
       </c>
       <c r="G4" t="s">
-        <v>126</v>
+        <v>174</v>
       </c>
       <c r="H4" t="s">
-        <v>150</v>
+        <v>206</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>172</v>
+        <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>58</v>
+        <v>84</v>
       </c>
       <c r="D5" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
       <c r="E5" t="s">
-        <v>93</v>
+        <v>126</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>149</v>
       </c>
       <c r="G5" t="s">
-        <v>127</v>
+        <v>175</v>
       </c>
       <c r="H5" t="s">
-        <v>151</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>35</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>82</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>150</v>
       </c>
       <c r="G6" t="s">
-        <v>128</v>
+        <v>176</v>
       </c>
       <c r="H6" t="s">
-        <v>152</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>104</v>
       </c>
       <c r="E7" t="s">
-        <v>90</v>
+        <v>128</v>
       </c>
       <c r="F7" t="s">
-        <v>110</v>
+        <v>51</v>
       </c>
       <c r="G7" t="s">
-        <v>129</v>
+        <v>177</v>
       </c>
       <c r="H7" t="s">
-        <v>153</v>
+        <v>209</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="B8" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C8" t="s">
-        <v>61</v>
+        <v>87</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="F8" t="s">
-        <v>111</v>
+        <v>51</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>178</v>
       </c>
       <c r="H8" t="s">
-        <v>154</v>
+        <v>210</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>38</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>62</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="E9" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="F9" t="s">
-        <v>112</v>
+        <v>151</v>
       </c>
       <c r="G9" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="H9" t="s">
-        <v>155</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>39</v>
+        <v>58</v>
       </c>
       <c r="C10" t="s">
-        <v>63</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>84</v>
+        <v>102</v>
       </c>
       <c r="E10" t="s">
-        <v>90</v>
+        <v>130</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="G10" t="s">
-        <v>132</v>
+        <v>180</v>
       </c>
       <c r="H10" t="s">
-        <v>156</v>
+        <v>212</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="C11" t="s">
-        <v>64</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E11" t="s">
-        <v>96</v>
+        <v>131</v>
       </c>
       <c r="F11" t="s">
-        <v>114</v>
+        <v>153</v>
       </c>
       <c r="G11" t="s">
-        <v>133</v>
+        <v>181</v>
       </c>
       <c r="H11" t="s">
-        <v>157</v>
+        <v>213</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>173</v>
+        <v>31</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
-        <v>174</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>79</v>
+        <v>108</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>131</v>
       </c>
       <c r="F12" t="s">
-        <v>113</v>
+        <v>153</v>
       </c>
       <c r="G12" t="s">
-        <v>175</v>
+        <v>182</v>
       </c>
       <c r="H12" t="s">
-        <v>176</v>
+        <v>214</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>32</v>
       </c>
       <c r="B13" t="s">
-        <v>42</v>
+        <v>61</v>
       </c>
       <c r="C13" t="s">
-        <v>65</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>79</v>
+        <v>109</v>
       </c>
       <c r="E13" t="s">
-        <v>90</v>
+        <v>132</v>
       </c>
       <c r="F13" t="s">
-        <v>115</v>
+        <v>154</v>
       </c>
       <c r="G13" t="s">
-        <v>134</v>
+        <v>183</v>
       </c>
       <c r="H13" t="s">
-        <v>158</v>
+        <v>215</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C14" t="s">
-        <v>66</v>
+        <v>93</v>
       </c>
       <c r="D14" t="s">
-        <v>82</v>
+        <v>109</v>
       </c>
       <c r="E14" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
       <c r="F14" t="s">
-        <v>116</v>
+        <v>154</v>
       </c>
       <c r="G14" t="s">
-        <v>135</v>
+        <v>184</v>
       </c>
       <c r="H14" t="s">
-        <v>159</v>
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
       <c r="C15" t="s">
-        <v>67</v>
+        <v>94</v>
       </c>
       <c r="D15" t="s">
-        <v>86</v>
+        <v>110</v>
       </c>
       <c r="E15" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="G15" t="s">
-        <v>136</v>
+        <v>185</v>
       </c>
       <c r="H15" t="s">
-        <v>160</v>
+        <v>216</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B16" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C16" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="D16" t="s">
-        <v>87</v>
+        <v>111</v>
       </c>
       <c r="E16" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="F16" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="G16" t="s">
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="H16" t="s">
-        <v>161</v>
+        <v>217</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>23</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
       <c r="D17" t="s">
-        <v>84</v>
+        <v>104</v>
       </c>
       <c r="E17" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="F17" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="G17" t="s">
-        <v>138</v>
+        <v>187</v>
       </c>
       <c r="H17" t="s">
-        <v>162</v>
+        <v>218</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B18" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D18" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="E18" t="s">
-        <v>101</v>
+        <v>114</v>
       </c>
       <c r="F18" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="G18" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="H18" t="s">
-        <v>163</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
-        <v>48</v>
+        <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D19" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="E19" t="s">
-        <v>102</v>
+        <v>113</v>
       </c>
       <c r="F19" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="G19" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
       <c r="H19" t="s">
-        <v>164</v>
+        <v>189</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>26</v>
+        <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D20" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="E20" t="s">
-        <v>103</v>
+        <v>114</v>
       </c>
       <c r="F20" t="s">
-        <v>29</v>
+        <v>138</v>
       </c>
       <c r="G20" t="s">
-        <v>141</v>
+        <v>159</v>
       </c>
       <c r="H20" t="s">
-        <v>165</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>27</v>
+        <v>11</v>
       </c>
       <c r="B21" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C21" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="E21" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="F21" t="s">
-        <v>122</v>
+        <v>139</v>
       </c>
       <c r="G21" t="s">
-        <v>142</v>
+        <v>160</v>
       </c>
       <c r="H21" t="s">
-        <v>166</v>
+        <v>192</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B22" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="C22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="D22" t="s">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="E22" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="F22" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="G22" t="s">
-        <v>143</v>
+        <v>161</v>
       </c>
       <c r="H22" t="s">
-        <v>167</v>
+        <v>193</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="B23" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C23" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D23" t="s">
-        <v>82</v>
+        <v>102</v>
       </c>
       <c r="E23" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="F23" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="G23" t="s">
-        <v>144</v>
+        <v>163</v>
       </c>
       <c r="H23" t="s">
-        <v>168</v>
+        <v>195</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
+        <v>15</v>
       </c>
       <c r="B24" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D24" t="s">
-        <v>82</v>
+        <v>103</v>
       </c>
       <c r="E24" t="s">
-        <v>106</v>
+        <v>119</v>
       </c>
       <c r="F24" t="s">
-        <v>123</v>
+        <v>54</v>
       </c>
       <c r="G24" t="s">
-        <v>145</v>
+        <v>164</v>
       </c>
       <c r="H24" t="s">
-        <v>169</v>
+        <v>196</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C25" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D25" t="s">
-        <v>79</v>
+        <v>101</v>
       </c>
       <c r="E25" t="s">
-        <v>90</v>
+        <v>117</v>
       </c>
       <c r="F25" t="s">
-        <v>41</v>
+        <v>141</v>
       </c>
       <c r="G25" t="s">
-        <v>146</v>
+        <v>162</v>
       </c>
       <c r="H25" t="s">
-        <v>170</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
+        <v>16</v>
       </c>
       <c r="B26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>104</v>
+      </c>
+      <c r="E26" t="s">
+        <v>120</v>
+      </c>
+      <c r="F26" t="s">
+        <v>20</v>
+      </c>
+      <c r="G26" t="s">
+        <v>165</v>
+      </c>
+      <c r="H26" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27" t="s">
+        <v>46</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" t="s">
+        <v>101</v>
+      </c>
+      <c r="E27" t="s">
+        <v>121</v>
+      </c>
+      <c r="F27" t="s">
+        <v>143</v>
+      </c>
+      <c r="G27" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" t="s">
+        <v>74</v>
+      </c>
+      <c r="D28" t="s">
+        <v>103</v>
+      </c>
+      <c r="E28" t="s">
+        <v>119</v>
+      </c>
+      <c r="F28" t="s">
         <v>54</v>
       </c>
-      <c r="C26" t="s">
+      <c r="G28" t="s">
+        <v>164</v>
+      </c>
+      <c r="H28" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" t="s">
+        <v>45</v>
+      </c>
+      <c r="C29" t="s">
+        <v>75</v>
+      </c>
+      <c r="D29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F29" t="s">
+        <v>20</v>
+      </c>
+      <c r="G29" t="s">
+        <v>165</v>
+      </c>
+      <c r="H29" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>18</v>
+      </c>
+      <c r="B30" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" t="s">
+        <v>101</v>
+      </c>
+      <c r="E30" t="s">
+        <v>122</v>
+      </c>
+      <c r="F30" t="s">
+        <v>144</v>
+      </c>
+      <c r="G30" t="s">
+        <v>167</v>
+      </c>
+      <c r="H30" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" t="s">
         <v>78</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E31" t="s">
+        <v>123</v>
+      </c>
+      <c r="F31" t="s">
+        <v>145</v>
+      </c>
+      <c r="G31" t="s">
+        <v>168</v>
+      </c>
+      <c r="H31" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" t="s">
         <v>79</v>
       </c>
-      <c r="E26" t="s">
-        <v>90</v>
-      </c>
-      <c r="F26" t="s">
-        <v>41</v>
-      </c>
-      <c r="G26" t="s">
-        <v>147</v>
-      </c>
-      <c r="H26" t="s">
+      <c r="D32" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" t="s">
+        <v>123</v>
+      </c>
+      <c r="F32" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" t="s">
+        <v>169</v>
+      </c>
+      <c r="H32" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+      <c r="B33" t="s">
+        <v>38</v>
+      </c>
+      <c r="C33" t="s">
+        <v>80</v>
+      </c>
+      <c r="D33" t="s">
+        <v>99</v>
+      </c>
+      <c r="E33" t="s">
+        <v>114</v>
+      </c>
+      <c r="F33" t="s">
+        <v>146</v>
+      </c>
+      <c r="G33" t="s">
+        <v>170</v>
+      </c>
+      <c r="H33" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>22</v>
+      </c>
+      <c r="B34" t="s">
+        <v>49</v>
+      </c>
+      <c r="C34" t="s">
+        <v>81</v>
+      </c>
+      <c r="D34" t="s">
+        <v>99</v>
+      </c>
+      <c r="E34" t="s">
+        <v>114</v>
+      </c>
+      <c r="F34" t="s">
+        <v>146</v>
+      </c>
+      <c r="G34" t="s">
         <v>171</v>
+      </c>
+      <c r="H34" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>36</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" t="s">
+        <v>97</v>
+      </c>
+      <c r="D35" t="s">
+        <v>112</v>
+      </c>
+      <c r="E35" t="s">
+        <v>135</v>
+      </c>
+      <c r="F35" t="s">
+        <v>51</v>
+      </c>
+      <c r="G35" t="s">
+        <v>188</v>
+      </c>
+      <c r="H35" t="s">
+        <v>219</v>
       </c>
     </row>
   </sheetData>

</xml_diff>